<commit_message>
tabela com nova atualização
</commit_message>
<xml_diff>
--- a/GUIL POINTS.xlsx
+++ b/GUIL POINTS.xlsx
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t>GUIL MEMROS</t>
-  </si>
-  <si>
-    <t>Points</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>PARNA COST</t>
   </si>
@@ -59,32 +53,32 @@
     <t>25 POINTS</t>
   </si>
   <si>
-    <t>WORD BOSS</t>
-  </si>
-  <si>
-    <t>INTRODUÇÃO: Pontos da guild (pdg) serve para priorizar os jogadores que estão mais participando nos eventos que exige colaboração da equipe,</t>
-  </si>
-  <si>
     <t>Points(PDG)</t>
   </si>
   <si>
-    <t>seja Word Boss ou simplesmente publicando algo no shopdaguild pra aumenta a verba da guild, aqueles q tiverem mais pontos tem mais prioridade sobre a venda e os itens vendido por preços promoçonais</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item publicado </t>
-  </si>
-  <si>
-    <t>no shopdaguild</t>
-  </si>
-  <si>
     <t>2 POINTS</t>
+  </si>
+  <si>
+    <t>Newgate</t>
+  </si>
+  <si>
+    <t>1 POINTS</t>
+  </si>
+  <si>
+    <t>3 POINTS</t>
+  </si>
+  <si>
+    <t>Item publicado NO SHOP</t>
+  </si>
+  <si>
+    <t>Word Boss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,20 +106,6 @@
       <charset val="177"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Andalus"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -133,22 +113,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color theme="5"/>
+      <name val="Baskerville Old Face"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Andalus"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Andalus"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Batang"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Andalus"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Baskerville Old Face"/>
+      <family val="1"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="4"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color rgb="FFC00000"/>
+      <name val="Andalus"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,31 +176,41 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor theme="2" tint="-0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkDown">
+        <bgColor theme="6" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkDown">
+        <bgColor theme="9" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -228,27 +257,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -316,15 +357,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>19115</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -347,8 +388,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2438400" y="1323975"/>
-          <a:ext cx="1733550" cy="390590"/>
+          <a:off x="2457450" y="2886076"/>
+          <a:ext cx="1733550" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -359,16 +400,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1708950</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>460482</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>13500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -391,8 +432,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2419350" y="3105150"/>
-          <a:ext cx="1728000" cy="374757"/>
+          <a:off x="2457450" y="3305176"/>
+          <a:ext cx="1728000" cy="485774"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -406,13 +447,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>19049</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>13499</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>450403</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>2729</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -435,8 +476,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2457449" y="3276600"/>
-          <a:ext cx="1728000" cy="374203"/>
+          <a:off x="2457449" y="4695826"/>
+          <a:ext cx="1728000" cy="440878"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -447,16 +488,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>476250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1718475</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>438151</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>13500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -479,8 +520,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2428875" y="2314576"/>
-          <a:ext cx="1728000" cy="381000"/>
+          <a:off x="2457450" y="3781425"/>
+          <a:ext cx="1728000" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -494,7 +535,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
@@ -523,8 +564,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2447924" y="2828925"/>
-          <a:ext cx="1728000" cy="383872"/>
+          <a:off x="2447924" y="4267200"/>
+          <a:ext cx="1728000" cy="421972"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -536,15 +577,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>9523</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>361948</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1728000</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3975</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -567,7 +608,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2438400" y="2171698"/>
+          <a:off x="2447925" y="2457448"/>
           <a:ext cx="1728000" cy="428627"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -580,15 +621,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1038226</xdr:colOff>
+      <xdr:colOff>1038225</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1076326</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>4596</xdr:rowOff>
+      <xdr:colOff>1362074</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>552450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -611,8 +652,96 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6257926" y="10991850"/>
-          <a:ext cx="1085850" cy="471321"/>
+          <a:off x="6257925" y="11096625"/>
+          <a:ext cx="1371599" cy="542925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>219076</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>379024</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2428876" y="2038351"/>
+          <a:ext cx="388548" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagem 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6629400" y="5476875"/>
+          <a:ext cx="3048000" cy="2733675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -887,16 +1016,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P38"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="A36" sqref="A36:O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="7" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="15.85546875" customWidth="1"/>
@@ -904,213 +1034,354 @@
     <col min="12" max="12" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="70.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-    </row>
-    <row r="3" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="9"/>
-    </row>
-    <row r="4" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:16" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="8">
+    <row r="1" spans="1:16" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+    </row>
+    <row r="2" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:16" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+    </row>
+    <row r="6" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="15"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+    <row r="8" spans="1:16" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="15"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="8">
+    <row r="9" spans="1:16" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="15"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+    <row r="10" spans="1:16" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="15"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="8">
+    <row r="11" spans="1:16" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="15"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="9">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+    <row r="12" spans="1:16" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="15"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="2:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="2:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="2:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="5:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="5:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="5:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="23" spans="5:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="5:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="5:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="5:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="5:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H29" s="11" t="s">
+    <row r="13" spans="1:16" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="16"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F14" s="16"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="K14" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="10.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F15" s="16"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F16" s="16"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="K16" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F17" s="16"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F18" s="16"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="K18" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="F19" s="16"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="K20" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+    </row>
+    <row r="25" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+    </row>
+    <row r="26" spans="1:17" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+    </row>
+    <row r="27" spans="1:17" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="10"/>
+    </row>
+    <row r="30" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E30" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I29" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="5:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E30" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="5:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E31" s="7" t="s">
+      <c r="I30" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E31" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="E32" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F32" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="E33" s="12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="5:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E32" s="7" t="s">
+      <c r="F33" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E33" s="7" t="s">
+    </row>
+    <row r="34" spans="1:15" ht="21.75" x14ac:dyDescent="0.5">
+      <c r="E34" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F34" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="5:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E34" s="7" t="s">
+    <row r="35" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E35" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F35" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="5:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E35" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
+    <row r="36" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+    </row>
+    <row r="37" spans="1:15" ht="210" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E38" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:O3"/>
-    <mergeCell ref="B2:O2"/>
+  <mergeCells count="5">
+    <mergeCell ref="A36:O37"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="A1:O5"/>
+    <mergeCell ref="B24:Q26"/>
+    <mergeCell ref="A24:A26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>